<commit_message>
Add files for 01-Excel\2
</commit_message>
<xml_diff>
--- a/01-Lesson-Plans/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/Excel_Playground_Starter.xlsx
+++ b/01-Lesson-Plans/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/Excel_Playground_Starter.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afhaque/TrilogyWork/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/2/Activities/01-Ins_ExcelPlayground/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8512a5b4b9cbd9d/UCB/temp/UCB-VIRT-DATA-PT-08-2023-U-LOLC/01-Lesson-Plans/01-Excel/2/Activities/01-Ins_ExcelPlayground/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_79800E530DF6EE7C2DDA7C133E6F23C10BAF778D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5DD3EFF-7F01-4700-98F9-B0A7F965088F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -101,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -197,6 +209,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -464,26 +479,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,7 +524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1</f>
         <v>1</v>
@@ -526,13 +541,19 @@
       <c r="E2">
         <v>92</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <f>AVERAGE(C2:E2)</f>
+        <v>87.666666666666671</v>
+      </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="3">
+        <f>SUM(F2:G2)</f>
+        <v>88.666666666666671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -548,13 +569,19 @@
       <c r="E3">
         <v>97</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F10" si="0">AVERAGE(C3:E3)</f>
+        <v>94</v>
+      </c>
       <c r="G3">
         <v>3</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H10" si="1">SUM(F3:G3)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -570,13 +597,19 @@
       <c r="E4">
         <v>84</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>89.333333333333329</v>
+      </c>
       <c r="G4">
         <v>4</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -592,13 +625,19 @@
       <c r="E5">
         <v>97</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="3">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -614,13 +653,19 @@
       <c r="E6">
         <v>83</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -636,13 +681,19 @@
       <c r="E7">
         <v>97</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>94.666666666666671</v>
+      </c>
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="3">
+        <f t="shared" si="1"/>
+        <v>95.666666666666671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -658,13 +709,19 @@
       <c r="E8">
         <v>93</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>90.666666666666671</v>
+      </c>
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="3">
+        <f t="shared" si="1"/>
+        <v>92.666666666666671</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -680,13 +737,19 @@
       <c r="E9">
         <v>97</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>89.333333333333329</v>
+      </c>
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="3">
+        <f t="shared" si="1"/>
+        <v>92.333333333333329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -702,47 +765,68 @@
       <c r="E10">
         <v>96</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>93.666666666666671</v>
+      </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>93.666666666666671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="6">
+        <f>AVERAGE(H2:H10)</f>
+        <v>92.259259259259252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="6">
+        <f>MEDIAN(H2:H10)</f>
+        <v>92.666666666666671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="6">
+        <f>MAX(H2:H10)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="6">
+        <f>MIN(H2:H10)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5">
+        <f>_xlfn.STDEV.P(H2:H10)</f>
+        <v>2.9638887442581567</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>